<commit_message>
Custom Employee Template Export
</commit_message>
<xml_diff>
--- a/public/DataEmployee/data-pegawai.xlsx
+++ b/public/DataEmployee/data-pegawai.xlsx
@@ -15,45 +15,27 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="13">
-  <si>
-    <t>maria</t>
-  </si>
-  <si>
-    <t>2023-12-29T16:03:36.000000Z</t>
-  </si>
-  <si>
-    <t>2023-12-31T02:14:31.000000Z</t>
-  </si>
-  <si>
-    <t>Zakia</t>
-  </si>
-  <si>
-    <t>2023-12-31T02:18:54.000000Z</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="7">
   <si>
     <t>Ananda Zakia Syahfitri</t>
   </si>
   <si>
-    <t>Kepala</t>
-  </si>
-  <si>
-    <t>2023-12-31T02:25:29.000000Z</t>
-  </si>
-  <si>
-    <t>ananda</t>
-  </si>
-  <si>
     <t>Sekretaris</t>
   </si>
   <si>
-    <t>2023-12-31T02:28:21.000000Z</t>
-  </si>
-  <si>
-    <t>sayang</t>
-  </si>
-  <si>
-    <t>2023-12-31T02:34:00.000000Z</t>
+    <t>2023-12-31T04:45:40.000000Z</t>
+  </si>
+  <si>
+    <t>Bima Sakti</t>
+  </si>
+  <si>
+    <t>Anggota</t>
+  </si>
+  <si>
+    <t>2023-12-31T04:55:18.000000Z</t>
+  </si>
+  <si>
+    <t>2023-12-31T04:56:47.000000Z</t>
   </si>
 </sst>
 </file>
@@ -393,7 +375,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:H6"/>
+  <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -403,7 +385,7 @@
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1">
-        <v>1</v>
+        <v>58</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -415,146 +397,94 @@
         <v>12345</v>
       </c>
       <c r="E1">
+        <v>1</v>
+      </c>
+      <c r="F1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G1" t="s">
         <v>2</v>
       </c>
-      <c r="F1">
+      <c r="H1" t="s">
         <v>2</v>
-      </c>
-      <c r="G1" t="s">
-        <v>1</v>
-      </c>
-      <c r="H1" t="s">
-        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:8">
       <c r="A2">
-        <v>2</v>
-      </c>
-      <c r="B2">
-        <v>1</v>
+        <v>59</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
       </c>
       <c r="C2">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D2">
-        <v>1</v>
+        <v>6789</v>
       </c>
       <c r="E2">
-        <v>1</v>
-      </c>
-      <c r="F2">
-        <v>1</v>
+        <v>3</v>
+      </c>
+      <c r="F2" t="s">
+        <v>4</v>
       </c>
       <c r="G2" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="H2" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:8">
       <c r="A3">
-        <v>3</v>
+        <v>60</v>
       </c>
       <c r="B3" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C3">
         <v>1</v>
       </c>
       <c r="D3">
-        <v>1</v>
+        <v>12345</v>
       </c>
       <c r="E3">
         <v>1</v>
       </c>
-      <c r="F3">
+      <c r="F3" t="s">
         <v>1</v>
       </c>
       <c r="G3" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="H3" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:8">
       <c r="A4">
-        <v>5</v>
+        <v>61</v>
       </c>
       <c r="B4" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C4">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D4">
+        <v>6789</v>
+      </c>
+      <c r="E4">
         <v>3</v>
       </c>
-      <c r="E4">
-        <v>2</v>
-      </c>
       <c r="F4" t="s">
+        <v>4</v>
+      </c>
+      <c r="G4" t="s">
         <v>6</v>
       </c>
-      <c r="G4" t="s">
-        <v>7</v>
-      </c>
       <c r="H4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8">
-      <c r="A5">
         <v>6</v>
-      </c>
-      <c r="B5" t="s">
-        <v>8</v>
-      </c>
-      <c r="C5">
-        <v>2</v>
-      </c>
-      <c r="D5">
-        <v>123456789</v>
-      </c>
-      <c r="E5">
-        <v>2</v>
-      </c>
-      <c r="F5" t="s">
-        <v>9</v>
-      </c>
-      <c r="G5" t="s">
-        <v>10</v>
-      </c>
-      <c r="H5" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8">
-      <c r="A6">
-        <v>7</v>
-      </c>
-      <c r="B6" t="s">
-        <v>11</v>
-      </c>
-      <c r="C6">
-        <v>1</v>
-      </c>
-      <c r="D6">
-        <v>1</v>
-      </c>
-      <c r="E6">
-        <v>1</v>
-      </c>
-      <c r="F6">
-        <v>1</v>
-      </c>
-      <c r="G6" t="s">
-        <v>12</v>
-      </c>
-      <c r="H6" t="s">
-        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>